<commit_message>
Cập nhật danh sách khách
</commit_message>
<xml_diff>
--- a/DSKH.xlsx
+++ b/DSKH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HNT24\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_render\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6D0050-421A-4F87-8D85-B0CDDBCE5F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1140DE5A-C29A-46B6-B9C5-50A4087618D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="683">
   <si>
     <t>STT</t>
   </si>
@@ -2078,6 +2078,15 @@
   </si>
   <si>
     <t>0100109106-011</t>
+  </si>
+  <si>
+    <t>KHTV.143</t>
+  </si>
+  <si>
+    <t>0315266142</t>
+  </si>
+  <si>
+    <t>Công ty cổ phần MP Logistics</t>
   </si>
 </sst>
 </file>
@@ -2239,17 +2248,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{72968E78-4D5E-40B5-8606-A1CA43B72489}"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2509,10 +2508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E243"/>
+  <dimension ref="A1:E244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
+      <selection activeCell="B243" sqref="B243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -5485,7 +5484,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="14">
-        <f t="shared" ref="A196:A243" si="3">+A195+1</f>
+        <f t="shared" ref="A196:A244" si="3">+A195+1</f>
         <v>195</v>
       </c>
       <c r="B196" s="20" t="s">
@@ -6203,9 +6202,24 @@
         <v>669</v>
       </c>
     </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" s="14">
+        <f t="shared" si="3"/>
+        <v>243</v>
+      </c>
+      <c r="B244" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="C244" s="21" t="s">
+        <v>681</v>
+      </c>
+      <c r="D244" s="19" t="s">
+        <v>680</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>